<commit_message>
Added retry scopes. Added delay for account search. Fixed "do_not_reply" emails
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://electrocomponents-my.sharepoint.com/personal/teofil_raicu_rsgroup_com/Documents/Documents/PO Processing Perfomer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A840AED7-AEDD-4571-924C-5444A87EE3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{159E7D1A-BF9B-49A8-ABA6-D8FEBA389C17}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{A840AED7-AEDD-4571-924C-5444A87EE3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FB3BA5A-3B41-487C-87E1-0A84FE01E6C5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,7 +242,7 @@
     <t>PO_IgnorePODuplicates</t>
   </si>
   <si>
-    <t>OrderManagement_PostDU_test</t>
+    <t>OrderManagement_PostDU</t>
   </si>
 </sst>
 </file>
@@ -759,7 +759,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4257,7 +4257,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4277,12 +4277,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4302,7 +4302,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Send SE and BRe email based on the country. If the PO number is not provided, use today's date
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://electrocomponents-my.sharepoint.com/personal/teofil_raicu_rsgroup_com/Documents/Documents/PO Processing Perfomer/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{A840AED7-AEDD-4571-924C-5444A87EE3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FB3BA5A-3B41-487C-87E1-0A84FE01E6C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515C6F91-2BBB-4281-8218-8F0FC48276ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -236,13 +236,28 @@
     <t>PO_SAP_IGNOREANYSAVING</t>
   </si>
   <si>
-    <t>PO_ErrorMailDestination</t>
-  </si>
-  <si>
     <t>PO_IgnorePODuplicates</t>
   </si>
   <si>
-    <t>OrderManagement_PostDU</t>
+    <t>PO_FR_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>PO_DE_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>PO_UK_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>FR_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>UK_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>DE_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>OrderManagement_PostDU_test</t>
   </si>
 </sst>
 </file>
@@ -453,10 +468,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -759,7 +770,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -809,7 +820,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -3008,10 +3019,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3268,14 +3279,28 @@
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
         <v>71</v>
       </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -4244,7 +4269,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed this bug: 97 "Article # was entered, but BOT was unable to enter the qty, hence manual intervention was done. Also the delivery date was not changed. Need to investigate, if it was because of new pop up"
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515C6F91-2BBB-4281-8218-8F0FC48276ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CC3810-F0A9-4989-9CCE-1F7F9C6780BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
     <t>DE_ErrorMailDestination</t>
   </si>
   <si>
-    <t>OrderManagement_PostDU_test</t>
+    <t>OrderManagement_PostDU</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4281,7 +4281,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="Control 2">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4301,12 +4301,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="Control 2"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="Control 1">
+        <control shapeId="1026" r:id="rId6" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4326,7 +4326,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="Control 1"/>
+        <control shapeId="1026" r:id="rId6" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
fixed changing the country in profile parameters
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CC3810-F0A9-4989-9CCE-1F7F9C6780BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802FF8B8-8766-4DA4-B4A5-A8D71EC7A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
     <t>DE_ErrorMailDestination</t>
   </si>
   <si>
-    <t>OrderManagement_PostDU</t>
+    <t>OrderManagement_PostDU_test</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4281,7 +4281,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4301,12 +4301,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4326,7 +4326,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
fixed search contact and clicking on display header details in the PO
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802FF8B8-8766-4DA4-B4A5-A8D71EC7A02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BD64EF-B7EE-4B8B-8159-0FC152B255C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
     <t>DE_ErrorMailDestination</t>
   </si>
   <si>
-    <t>OrderManagement_PostDU_test</t>
+    <t>OrderManagement_PostDU</t>
   </si>
 </sst>
 </file>
@@ -4281,7 +4281,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="Control 2">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4301,12 +4301,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="Control 2"/>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="Control 1">
+        <control shapeId="1026" r:id="rId6" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4326,7 +4326,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="Control 1"/>
+        <control shapeId="1026" r:id="rId6" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
update create contact person for GB
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30BD64EF-B7EE-4B8B-8159-0FC152B255C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B01937-9D35-4819-9DC8-B614D17E5819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -245,19 +245,19 @@
     <t>PO_DE_ErrorMailDestination</t>
   </si>
   <si>
-    <t>PO_UK_ErrorMailDestination</t>
-  </si>
-  <si>
     <t>FR_ErrorMailDestination</t>
   </si>
   <si>
-    <t>UK_ErrorMailDestination</t>
-  </si>
-  <si>
     <t>DE_ErrorMailDestination</t>
   </si>
   <si>
     <t>OrderManagement_PostDU</t>
+  </si>
+  <si>
+    <t>GB_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>PO_GB_ErrorMailDestination</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -820,7 +820,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -3022,7 +3022,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3279,7 +3279,7 @@
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
         <v>72</v>
@@ -3287,15 +3287,15 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Fixed false popup appear
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B01937-9D35-4819-9DC8-B614D17E5819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976EBC57-666E-45ED-BFAD-0889CE68F861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -251,13 +251,13 @@
     <t>DE_ErrorMailDestination</t>
   </si>
   <si>
-    <t>OrderManagement_PostDU</t>
-  </si>
-  <si>
     <t>GB_ErrorMailDestination</t>
   </si>
   <si>
     <t>PO_GB_ErrorMailDestination</t>
+  </si>
+  <si>
+    <t>OrderManagement_PostDU_GB</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -820,7 +820,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -3287,10 +3287,10 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
         <v>76</v>
-      </c>
-      <c r="B29" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
@@ -4281,7 +4281,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4301,12 +4301,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4326,7 +4326,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fixed morning bugs and searches
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\C0999718\Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42905A6B-61AB-4084-8F63-53D4E0BC67BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AA09F6-5821-40FD-8902-DAA670CDC94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -257,10 +257,10 @@
     <t>PO_GB_ErrorMailDestination</t>
   </si>
   <si>
-    <t>OrderManagement_PostDU_FR</t>
-  </si>
-  <si>
     <t>PO_SAPCredential2</t>
+  </si>
+  <si>
+    <t>OrderManagement_PostDU_GB</t>
   </si>
 </sst>
 </file>
@@ -381,9 +381,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:rowOff>95250</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -431,9 +431,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>209550</xdr:colOff>
+          <xdr:colOff>257175</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>69850</xdr:rowOff>
+          <xdr:rowOff>95250</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -772,16 +772,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -823,13 +823,13 @@
         <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -839,7 +839,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1861,12 +1861,12 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1903,7 +1903,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2028,7 +2028,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3024,16 +3024,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="44.54296875" customWidth="1"/>
-    <col min="2" max="2" width="45.54296875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3157,7 +3157,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -4284,7 +4284,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4295,21 +4295,21 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>12</xdr:row>
-                <xdr:rowOff>69850</xdr:rowOff>
+                <xdr:rowOff>95250</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4320,16 +4320,16 @@
               </from>
               <to>
                 <xdr:col>0</xdr:col>
-                <xdr:colOff>209550</xdr:colOff>
+                <xdr:colOff>257175</xdr:colOff>
                 <xdr:row>12</xdr:row>
-                <xdr:rowOff>69850</xdr:rowOff>
+                <xdr:rowOff>95250</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fixed issues mentioned on 29/10/2025
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RSComponentsPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9638FDE8-60A4-467C-B1ED-34BFA691531D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29B6181-591C-4432-8743-DD518D3F0B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23160" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4284,7 +4284,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="Control 1">
+        <control shapeId="1026" r:id="rId4" name="Control 2">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4304,12 +4304,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+        <control shapeId="1026" r:id="rId4" name="Control 2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="Control 2">
+        <control shapeId="1025" r:id="rId6" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
@@ -4329,7 +4329,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+        <control shapeId="1025" r:id="rId6" name="Control 1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>